<commit_message>
Added value to the Excel import report table.
</commit_message>
<xml_diff>
--- a/conf-core/src/test/resources/dataloader/properties-fail-delete.test.xlsx
+++ b/conf-core/src/test/resources/dataloader/properties-fail-delete.test.xlsx
@@ -510,9 +510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>